<commit_message>
Adding cost by component breakdown of LCOH and saving results to CSV
</commit_message>
<xml_diff>
--- a/Parameters/demand_parameters.xlsx
+++ b/Parameters/demand_parameters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioxfordnexus-my.sharepoint.com/personal/hert5576_ox_ac_uk/Documents/CCG/GEOH2/ETH Hydrogen Collaboration/Inputs and results v12 2023-09-05/kenya-local-derisked/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioxfordnexus-my.sharepoint.com/personal/hert5576_ox_ac_uk/Documents/CCG/GEOH2/ETH Hydrogen Collaboration/Inputs and results v11 2023-09-01/namibia-export-derisked/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{FCC86708-CBAF-6A47-8F9C-BE94266B62AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E1FFCF4-18CB-42BC-948D-1553B700A847}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{CE9DFDE7-1E8E-CC40-8F9D-55162186CABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F843754-EE93-4B24-B1AF-19130F7F545D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{1EFB3969-2EEE-7045-9FD0-00480E0E3DAF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1EFB3969-2EEE-7045-9FD0-00480E0E3DAF}"/>
   </bookViews>
   <sheets>
     <sheet name="Demand centers" sheetId="2" r:id="rId1"/>
@@ -20,16 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -55,7 +45,7 @@
     <t>Demand state</t>
   </si>
   <si>
-    <t>Olkaria</t>
+    <t>Lüderitz</t>
   </si>
 </sst>
 </file>
@@ -429,22 +419,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A21CD761-0C02-5F48-878C-D5E4B46C4E1D}">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.375" customWidth="1"/>
-    <col min="2" max="2" width="16.375" customWidth="1"/>
-    <col min="3" max="3" width="20.125" customWidth="1"/>
-    <col min="4" max="4" width="22.375" customWidth="1"/>
-    <col min="5" max="5" width="29.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.296875" customWidth="1"/>
+    <col min="2" max="2" width="16.296875" customWidth="1"/>
+    <col min="3" max="3" width="20.19921875" customWidth="1"/>
+    <col min="4" max="4" width="22.296875" customWidth="1"/>
+    <col min="5" max="5" width="29.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -461,203 +451,22 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="1">
-        <v>-0.85539676297365497</v>
+        <v>-26.642877645011101</v>
       </c>
       <c r="C2" s="1">
-        <v>36.317985788964002</v>
+        <v>15.1439290700957</v>
       </c>
       <c r="D2" s="3">
-        <f>52*1000000</f>
-        <v>52000000</v>
+        <v>54000000</v>
       </c>
       <c r="E2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="3"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="3"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="3"/>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="3"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="3"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="3"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="3"/>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="3"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="3"/>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="3"/>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="3"/>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="3"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="3"/>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="3"/>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="3"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="3"/>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="3"/>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="3"/>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="3"/>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="3"/>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>